<commit_message>
- 【Nuget】版本更新到1.4.14 - 【重构】大量重构  - 移除部分未使用的代码  - 将TemplateFileInfo重命名为ExportFileInfo  - 将IExporterByTemplate接口拆分为4个接口：IExportListFileByTemplate, IExportListStringByTemplate, IExportStringByTemplate, IExportFileByTemplate，并修改相关实现  - 重构ImportHelper部分代码 - 【导入】修复导入Excel时表头设置的问题，已对此编写单元测试，见【产品信息导入】 - 【完善】编写ExportAsByteArray对于DataTable的单元测试，ExportWordFileByTemplate_Test
</commit_message>
<xml_diff>
--- a/src/Magicodes.ExporterAndImporter.Tests/TestFiles/Import/产品导入模板.xlsx
+++ b/src/Magicodes.ExporterAndImporter.Tests/TestFiles/Import/产品导入模板.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1D09EE-709C-4F34-9808-1D844ACBF26B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCD792F-08C1-4E6D-A920-B469C422FAC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -504,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A2:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="D13" sqref="D12:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -518,153 +519,111 @@
     <col min="15" max="15" width="15.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>123123</v>
-      </c>
-      <c r="B2">
-        <v>1212</v>
-      </c>
-      <c r="C2">
-        <v>12</v>
-      </c>
-      <c r="D2">
-        <v>1231</v>
-      </c>
-      <c r="E2">
-        <v>1234124</v>
-      </c>
-      <c r="F2">
-        <v>123123</v>
-      </c>
-      <c r="G2">
-        <v>1231</v>
-      </c>
-      <c r="H2">
-        <v>12412</v>
-      </c>
-      <c r="I2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2">
-        <v>20</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="3">
-        <f ca="1">TODAY()</f>
-        <v>43726</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="4" t="str">
-        <f>IF(MOD(MID(N2,17,1),2)=1,"男","女")</f>
-        <v>女</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>123123</v>
       </c>
       <c r="B3">
-        <v>12312312</v>
+        <v>1212</v>
       </c>
       <c r="C3">
-        <v>12123</v>
+        <v>12</v>
       </c>
       <c r="D3">
-        <v>12312412</v>
+        <v>1231</v>
       </c>
       <c r="E3">
-        <v>12312314</v>
+        <v>1234124</v>
       </c>
       <c r="F3">
-        <v>123124</v>
+        <v>123123</v>
       </c>
       <c r="G3">
         <v>1231</v>
       </c>
       <c r="H3">
-        <v>123513</v>
+        <v>12412</v>
       </c>
       <c r="I3" t="s">
         <v>10</v>
       </c>
       <c r="J3">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M3" s="3">
         <f ca="1">TODAY()</f>
-        <v>43726</v>
+        <v>43805</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" s="4" t="str">
+        <f>IF(MOD(MID(N3,17,1),2)=1,"男","女")</f>
+        <v>女</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>123123</v>
       </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
+      <c r="B4">
+        <v>12312312</v>
+      </c>
+      <c r="C4">
+        <v>12123</v>
       </c>
       <c r="D4">
         <v>12312412</v>
@@ -682,10 +641,10 @@
         <v>123513</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="J4">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>15</v>
@@ -694,8 +653,8 @@
         <v>16</v>
       </c>
       <c r="M4" s="3">
-        <f t="shared" ref="M4:M7" ca="1" si="0">TODAY()</f>
-        <v>43726</v>
+        <f ca="1">TODAY()</f>
+        <v>43805</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -703,10 +662,10 @@
         <v>123123</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>12312412</v>
@@ -736,13 +695,13 @@
         <v>16</v>
       </c>
       <c r="M5" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>43726</v>
+        <f t="shared" ref="M5:M8" ca="1" si="0">TODAY()</f>
+        <v>43805</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>28</v>
+      <c r="A6">
+        <v>123123</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -766,10 +725,10 @@
         <v>123513</v>
       </c>
       <c r="I6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="J6">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>15</v>
@@ -779,12 +738,12 @@
       </c>
       <c r="M6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>43726</v>
+        <v>43805</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
@@ -808,7 +767,10 @@
         <v>123513</v>
       </c>
       <c r="I7" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="J7">
+        <v>52</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>15</v>
@@ -818,16 +780,55 @@
       </c>
       <c r="M7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>43726</v>
+        <v>43805</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8">
+        <v>12312412</v>
+      </c>
+      <c r="E8">
+        <v>12312314</v>
+      </c>
+      <c r="F8">
+        <v>123124</v>
+      </c>
+      <c r="G8">
+        <v>1231</v>
+      </c>
+      <c r="H8">
+        <v>123513</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>43805</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" sqref="L1:L7" xr:uid="{90061FCE-F949-4071-A206-8FCABBFDE82B}">
+    <dataValidation type="list" sqref="L2:L8" xr:uid="{90061FCE-F949-4071-A206-8FCABBFDE82B}">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="K1:K7" xr:uid="{D223E661-8643-415F-96E7-01981C896EC2}">
+    <dataValidation type="list" sqref="K2:K8" xr:uid="{D223E661-8643-415F-96E7-01981C896EC2}">
       <formula1>"第一,第二"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
- **【Nuget】版本更新到2.1.3** - **【Excel导入】修复GUID类型的问题。问题见（<https://github.com/dotnetcore/Magicodes.IE/issues/44>）。**
</commit_message>
<xml_diff>
--- a/src/Magicodes.ExporterAndImporter.Tests/TestFiles/Import/产品导入模板.xlsx
+++ b/src/Magicodes.ExporterAndImporter.Tests/TestFiles/Import/产品导入模板.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCD792F-08C1-4E6D-A920-B469C422FAC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7EB429-6E11-4D2D-965A-BB20ABF16DA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t>产品代码</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -139,6 +139,38 @@
   <si>
     <t>1231 23</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ProductIdTest1</t>
+  </si>
+  <si>
+    <t>ProductIdTest2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C2EE3694-959A-4A87-BC8C-4003F6576352</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C2EE3694-959A-4A87-BC8C-4003F6576353</t>
+  </si>
+  <si>
+    <t>C2EE3694-959A-4A87-BC8C-4003F6576354</t>
+  </si>
+  <si>
+    <t>C2EE3694-959A-4A87-BC8C-4003F6576355</t>
+  </si>
+  <si>
+    <t>C2EE3694-959A-4A87-BC8C-4003F6576356</t>
+  </si>
+  <si>
+    <t>C2EE3694-959A-4A87-BC8C-4003F6576357</t>
+  </si>
+  <si>
+    <t>C2EE3694-959A-4A87-BC8C-4003F6576358</t>
+  </si>
+  <si>
+    <t>C2EE3694-959A-4A87-BC8C-4003F6576359</t>
   </si>
 </sst>
 </file>
@@ -505,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:O8"/>
+  <dimension ref="A2:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D12:D13"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -517,9 +549,11 @@
     <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23.75" customWidth="1"/>
     <col min="15" max="15" width="15.375" customWidth="1"/>
+    <col min="16" max="16" width="40" customWidth="1"/>
+    <col min="17" max="17" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -565,8 +599,14 @@
       <c r="O2" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="P2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>123123</v>
       </c>
@@ -605,7 +645,7 @@
       </c>
       <c r="M3" s="3">
         <f ca="1">TODAY()</f>
-        <v>43805</v>
+        <v>43896</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>27</v>
@@ -614,8 +654,14 @@
         <f>IF(MOD(MID(N3,17,1),2)=1,"男","女")</f>
         <v>女</v>
       </c>
+      <c r="P3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>123123</v>
       </c>
@@ -654,10 +700,16 @@
       </c>
       <c r="M4" s="3">
         <f ca="1">TODAY()</f>
-        <v>43805</v>
+        <v>43896</v>
+      </c>
+      <c r="P4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>123123</v>
       </c>
@@ -696,10 +748,16 @@
       </c>
       <c r="M5" s="3">
         <f t="shared" ref="M5:M8" ca="1" si="0">TODAY()</f>
-        <v>43805</v>
+        <v>43896</v>
+      </c>
+      <c r="P5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>123123</v>
       </c>
@@ -738,10 +796,13 @@
       </c>
       <c r="M6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>43805</v>
+        <v>43896</v>
+      </c>
+      <c r="P6" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -780,10 +841,13 @@
       </c>
       <c r="M7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>43805</v>
+        <v>43896</v>
+      </c>
+      <c r="P7" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -819,7 +883,10 @@
       </c>
       <c r="M8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>43805</v>
+        <v>43896</v>
+      </c>
+      <c r="P8" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>